<commit_message>
added script to remove ANISOU from PDB files for interfacea recognition
</commit_message>
<xml_diff>
--- a/data/candidates.xlsx
+++ b/data/candidates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tneijen/Documents/Project/Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tneijen/Documents/gitdir/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97977F9C-9A2A-BD4B-8830-5826649A6132}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862D94C9-84E2-834B-A762-D56AADCC43EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11040" yWindow="460" windowWidth="24480" windowHeight="19240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{34E8DE18-1D87-1F47-8DFF-EC8DA429B9F9}" name="clash_list" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/tneijen/Documents/Project/Dataset/EM-PDB/clash_list.csv" decimal="," thousands=".">
+    <textPr sourceFile="/Users/tneijen/Documents/Project/Dataset/EM-PDB/clash_list.csv" decimal="," thousands=".">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="287">
   <si>
     <t>EMDB ID</t>
   </si>
@@ -902,6 +902,12 @@
   </si>
   <si>
     <t xml:space="preserve">6qg5.pdb </t>
+  </si>
+  <si>
+    <t>contains DNA</t>
+  </si>
+  <si>
+    <t>contains ANISOU which shoulc be removed, after removal classes = 77</t>
   </si>
 </sst>
 </file>
@@ -1480,11 +1486,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="2" xr16:uid="{DEC0D320-18C7-404B-BFD2-50D03D5167B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="2" xr16:uid="{DEC0D320-18C7-404B-BFD2-50D03D5167B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2685,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203E3033-B15E-BD4D-9992-052B94783655}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:E32"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2697,7 +2703,7 @@
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>247</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -2718,8 +2724,11 @@
       <c r="E2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -2732,8 +2741,11 @@
       <c r="E3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -2747,7 +2759,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -2760,8 +2772,11 @@
       <c r="E5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>218</v>
       </c>
@@ -2774,8 +2789,11 @@
       <c r="E6" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -2789,7 +2807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>220</v>
       </c>
@@ -2803,7 +2821,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>221</v>
       </c>
@@ -2817,7 +2835,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>222</v>
       </c>
@@ -2831,7 +2849,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>223</v>
       </c>
@@ -2845,7 +2863,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -2859,7 +2877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -2873,7 +2891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>226</v>
       </c>
@@ -2887,7 +2905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>227</v>
       </c>
@@ -2901,7 +2919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
added new higher resolution cryo-EM structures to the candidate list
</commit_message>
<xml_diff>
--- a/data/candidates.xlsx
+++ b/data/candidates.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tneijen/Documents/gitdir/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862D94C9-84E2-834B-A762-D56AADCC43EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFCAE92-9AD4-8242-A334-683925B257ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="460" windowWidth="24480" windowHeight="19240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="3720" windowWidth="24480" windowHeight="19240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="candidates" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="potential 5-8 angstrom" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="clash_list_1" localSheetId="1">Sheet2!$D$2:$E$36</definedName>
+    <definedName name="clashes" localSheetId="3">'potential 5-8 angstrom'!$E$1:$F$176</definedName>
     <definedName name="clashes" localSheetId="1">Sheet2!$A$2:$B$34</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -43,11 +45,19 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" xr16:uid="{EBF0FFD7-3D05-3748-A6E2-F97DBDCB6DE6}" name="clashes1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/tneijen/Documents/Project/Dataset/5-8reso/clashes.csv" decimal="," thousands=".">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="738">
   <si>
     <t>EMDB ID</t>
   </si>
@@ -904,17 +914,1370 @@
     <t xml:space="preserve">6qg5.pdb </t>
   </si>
   <si>
+    <t>empty file</t>
+  </si>
+  <si>
     <t>contains DNA</t>
   </si>
   <si>
-    <t>contains ANISOU which shoulc be removed, after removal classes = 77</t>
+    <t>after removal of all HOH and HETATM contained 2</t>
+  </si>
+  <si>
+    <t>file contains ANISOU which need to be removed, after removal, clash = 77</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>6 chains which contain nonbonded parts and  ATP</t>
+  </si>
+  <si>
+    <t>18 chains</t>
+  </si>
+  <si>
+    <t>18 chains elongated structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 chains, floating alpha helices with bound proteins. </t>
+  </si>
+  <si>
+    <t>6uby</t>
+  </si>
+  <si>
+    <t>PDB</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>6uc0</t>
+  </si>
+  <si>
+    <t>6k9k</t>
+  </si>
+  <si>
+    <t>7.82</t>
+  </si>
+  <si>
+    <t>6pwv</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>6upl</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>6olj</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>6pto</t>
+  </si>
+  <si>
+    <t>6kw3</t>
+  </si>
+  <si>
+    <t>7.13</t>
+  </si>
+  <si>
+    <t>6kw4</t>
+  </si>
+  <si>
+    <t>7.55</t>
+  </si>
+  <si>
+    <t>6rkw</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>6pas</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>6pvo</t>
+  </si>
+  <si>
+    <t>5.18</t>
+  </si>
+  <si>
+    <t>6sb2</t>
+  </si>
+  <si>
+    <t>6q0t</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>6r7i</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>6r7n</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>6qc9</t>
+  </si>
+  <si>
+    <t>6rxx</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>6nr8</t>
+  </si>
+  <si>
+    <t>6nra</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>6myx</t>
+  </si>
+  <si>
+    <t>6nme</t>
+  </si>
+  <si>
+    <t>5.67</t>
+  </si>
+  <si>
+    <t>6n7k</t>
+  </si>
+  <si>
+    <t>6n7g</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>6jma</t>
+  </si>
+  <si>
+    <t>6j4w</t>
+  </si>
+  <si>
+    <t>7.9</t>
+  </si>
+  <si>
+    <t>6ahf</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>6hms</t>
+  </si>
+  <si>
+    <t>6i7o</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>6irf</t>
+  </si>
+  <si>
+    <t>6n8t</t>
+  </si>
+  <si>
+    <t>6i27</t>
+  </si>
+  <si>
+    <t>6mj2</t>
+  </si>
+  <si>
+    <t>6.36</t>
+  </si>
+  <si>
+    <t>6gyk</t>
+  </si>
+  <si>
+    <t>6gym</t>
+  </si>
+  <si>
+    <t>6n1q</t>
+  </si>
+  <si>
+    <t>5.16</t>
+  </si>
+  <si>
+    <t>6mmm</t>
+  </si>
+  <si>
+    <t>6.84</t>
+  </si>
+  <si>
+    <t>6mmt</t>
+  </si>
+  <si>
+    <t>7.46</t>
+  </si>
+  <si>
+    <t>6hqa</t>
+  </si>
+  <si>
+    <t>6ah0</t>
+  </si>
+  <si>
+    <t>6hcq</t>
+  </si>
+  <si>
+    <t>6hiv</t>
+  </si>
+  <si>
+    <t>6a5t</t>
+  </si>
+  <si>
+    <t>6ed3</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>5z56</t>
+  </si>
+  <si>
+    <t>6h58</t>
+  </si>
+  <si>
+    <t>6fvv</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>6acg</t>
+  </si>
+  <si>
+    <t>6ejf</t>
+  </si>
+  <si>
+    <t>6dqz</t>
+  </si>
+  <si>
+    <t>6.01</t>
+  </si>
+  <si>
+    <t>6dbl</t>
+  </si>
+  <si>
+    <t>5vft</t>
+  </si>
+  <si>
+    <t>6d80</t>
+  </si>
+  <si>
+    <t>6g2i</t>
+  </si>
+  <si>
+    <t>5ywb</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5oqm</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>5zfu</t>
+  </si>
+  <si>
+    <t>5zam</t>
+  </si>
+  <si>
+    <t>6bjs</t>
+  </si>
+  <si>
+    <t>6c05</t>
+  </si>
+  <si>
+    <t>5.15</t>
+  </si>
+  <si>
+    <t>6c06</t>
+  </si>
+  <si>
+    <t>6fik</t>
+  </si>
+  <si>
+    <t>6ca0</t>
+  </si>
+  <si>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t>6bf7</t>
+  </si>
+  <si>
+    <t>6c3p</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>6f38</t>
+  </si>
+  <si>
+    <t>6f42</t>
+  </si>
+  <si>
+    <t>5y5z</t>
+  </si>
+  <si>
+    <t>6b7z</t>
+  </si>
+  <si>
+    <t>6bu9</t>
+  </si>
+  <si>
+    <t>5ydz</t>
+  </si>
+  <si>
+    <t>5.8Å</t>
+  </si>
+  <si>
+    <t>5ye2</t>
+  </si>
+  <si>
+    <t>6emk</t>
+  </si>
+  <si>
+    <t>7.9Å</t>
+  </si>
+  <si>
+    <t>6eny</t>
+  </si>
+  <si>
+    <t>5vvr</t>
+  </si>
+  <si>
+    <t>5vvs</t>
+  </si>
+  <si>
+    <t>6.4Å</t>
+  </si>
+  <si>
+    <t>6b5b</t>
+  </si>
+  <si>
+    <t>5.2Å</t>
+  </si>
+  <si>
+    <t>5oam</t>
+  </si>
+  <si>
+    <t>5.5Å</t>
+  </si>
+  <si>
+    <t>5ocu</t>
+  </si>
+  <si>
+    <t>6awc</t>
+  </si>
+  <si>
+    <t>5m50</t>
+  </si>
+  <si>
+    <t>5.3Å</t>
+  </si>
+  <si>
+    <t>8Å</t>
+  </si>
+  <si>
+    <t>5nd2</t>
+  </si>
+  <si>
+    <t>5nd3</t>
+  </si>
+  <si>
+    <t>6.1Å</t>
+  </si>
+  <si>
+    <t>5nd7</t>
+  </si>
+  <si>
+    <t>5y3r</t>
+  </si>
+  <si>
+    <t>6.6Å</t>
+  </si>
+  <si>
+    <t>5vh9</t>
+  </si>
+  <si>
+    <t>7.7Å</t>
+  </si>
+  <si>
+    <t>5vhn</t>
+  </si>
+  <si>
+    <t>7.3Å</t>
+  </si>
+  <si>
+    <t>5vhp</t>
+  </si>
+  <si>
+    <t>5vhr</t>
+  </si>
+  <si>
+    <t>5vhf</t>
+  </si>
+  <si>
+    <t>5.7Å</t>
+  </si>
+  <si>
+    <t>5vhh</t>
+  </si>
+  <si>
+    <t>5vhi</t>
+  </si>
+  <si>
+    <t>6.8Å</t>
+  </si>
+  <si>
+    <t>5w9n</t>
+  </si>
+  <si>
+    <t>5Å</t>
+  </si>
+  <si>
+    <t>5wcb</t>
+  </si>
+  <si>
+    <t>6Å</t>
+  </si>
+  <si>
+    <t>5oej</t>
+  </si>
+  <si>
+    <t>5wen</t>
+  </si>
+  <si>
+    <t>5nss</t>
+  </si>
+  <si>
+    <t>5mdx</t>
+  </si>
+  <si>
+    <t>5viy</t>
+  </si>
+  <si>
+    <t>6.2Å</t>
+  </si>
+  <si>
+    <t>5no3</t>
+  </si>
+  <si>
+    <t>5.16Å</t>
+  </si>
+  <si>
+    <t>5nrl</t>
+  </si>
+  <si>
+    <t>7.2Å</t>
+  </si>
+  <si>
+    <t>5np0</t>
+  </si>
+  <si>
+    <t>5np1</t>
+  </si>
+  <si>
+    <t>5u05</t>
+  </si>
+  <si>
+    <t>5uz4</t>
+  </si>
+  <si>
+    <t>5n61</t>
+  </si>
+  <si>
+    <t>6.9Å</t>
+  </si>
+  <si>
+    <t>5gpn</t>
+  </si>
+  <si>
+    <t>5.4Å</t>
+  </si>
+  <si>
+    <t>5n60</t>
+  </si>
+  <si>
+    <t>5n5z</t>
+  </si>
+  <si>
+    <t>5n5y</t>
+  </si>
+  <si>
+    <t>5ln3</t>
+  </si>
+  <si>
+    <t>5mqf</t>
+  </si>
+  <si>
+    <t>5.9Å</t>
+  </si>
+  <si>
+    <t>5wvi</t>
+  </si>
+  <si>
+    <t>6.3Å</t>
+  </si>
+  <si>
+    <t>5up2</t>
+  </si>
+  <si>
+    <t>5mpb</t>
+  </si>
+  <si>
+    <t>7.8Å</t>
+  </si>
+  <si>
+    <t>6ptn</t>
+  </si>
+  <si>
+    <t>5u1f</t>
+  </si>
+  <si>
+    <t>5h7i</t>
+  </si>
+  <si>
+    <t>7.1Å</t>
+  </si>
+  <si>
+    <t>5t4o</t>
+  </si>
+  <si>
+    <t>5tzs</t>
+  </si>
+  <si>
+    <t>5.1Å</t>
+  </si>
+  <si>
+    <t>5grs</t>
+  </si>
+  <si>
+    <t>5jbh</t>
+  </si>
+  <si>
+    <t>5.34Å</t>
+  </si>
+  <si>
+    <t>5jb3</t>
+  </si>
+  <si>
+    <t>5lqx</t>
+  </si>
+  <si>
+    <t>5lmp</t>
+  </si>
+  <si>
+    <t>5.35Å</t>
+  </si>
+  <si>
+    <t>5lms</t>
+  </si>
+  <si>
+    <t>5j7y</t>
+  </si>
+  <si>
+    <t>6.7Å</t>
+  </si>
+  <si>
+    <t>5j8k</t>
+  </si>
+  <si>
+    <t>5j4z</t>
+  </si>
+  <si>
+    <t>5gsy</t>
+  </si>
+  <si>
+    <t>7Å</t>
+  </si>
+  <si>
+    <t>5fkx</t>
+  </si>
+  <si>
+    <t>5ldx</t>
+  </si>
+  <si>
+    <t>5.6Å</t>
+  </si>
+  <si>
+    <t>5hnw</t>
+  </si>
+  <si>
+    <t>5kem</t>
+  </si>
+  <si>
+    <t>5khr</t>
+  </si>
+  <si>
+    <t>5hnx</t>
+  </si>
+  <si>
+    <t>5hny</t>
+  </si>
+  <si>
+    <t>5jpq</t>
+  </si>
+  <si>
+    <t>5g5p</t>
+  </si>
+  <si>
+    <t>5kne</t>
+  </si>
+  <si>
+    <t>5.64Å</t>
+  </si>
+  <si>
+    <t>5l9t</t>
+  </si>
+  <si>
+    <t>5g4f</t>
+  </si>
+  <si>
+    <t>5k0y</t>
+  </si>
+  <si>
+    <t>5kbt</t>
+  </si>
+  <si>
+    <t>5kbu</t>
+  </si>
+  <si>
+    <t>5k1h</t>
+  </si>
+  <si>
+    <t>5vov</t>
+  </si>
+  <si>
+    <t>5kk2</t>
+  </si>
+  <si>
+    <t>5fwp</t>
+  </si>
+  <si>
+    <t>5fwm</t>
+  </si>
+  <si>
+    <t>5jm0</t>
+  </si>
+  <si>
+    <t>5iy9</t>
+  </si>
+  <si>
+    <t>5iy8</t>
+  </si>
+  <si>
+    <t>5iya</t>
+  </si>
+  <si>
+    <t>5fxh</t>
+  </si>
+  <si>
+    <t>3jcr</t>
+  </si>
+  <si>
+    <t>5i1m</t>
+  </si>
+  <si>
+    <t>3jcg</t>
+  </si>
+  <si>
+    <t>7.06Å</t>
+  </si>
+  <si>
+    <t>3jch</t>
+  </si>
+  <si>
+    <t>3jcm</t>
+  </si>
+  <si>
+    <t>5flc</t>
+  </si>
+  <si>
+    <t>5fj6</t>
+  </si>
+  <si>
+    <t>5fkw</t>
+  </si>
+  <si>
+    <t>4ue4</t>
+  </si>
+  <si>
+    <t>5a5t</t>
+  </si>
+  <si>
+    <t>3jaq</t>
+  </si>
+  <si>
+    <t>3j82</t>
+  </si>
+  <si>
+    <t>3j95</t>
+  </si>
+  <si>
+    <t>7.6Å</t>
+  </si>
+  <si>
+    <t>3j96</t>
+  </si>
+  <si>
+    <t>4uxo</t>
+  </si>
+  <si>
+    <t>4uxp</t>
+  </si>
+  <si>
+    <t>4uxr</t>
+  </si>
+  <si>
+    <t>4uy0</t>
+  </si>
+  <si>
+    <t>4uqq</t>
+  </si>
+  <si>
+    <t>3j5m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3j5m.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3j82.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3j95.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3j96.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3jaq.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3jcg.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3jch.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3jcm.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3jcr.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4ue4.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4uqq.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4uxo.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4uxp.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4uxr.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4uy0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5a5t.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fj6.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fkw.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fkx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5flc.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fwm.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fwp.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5fxh.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5g4f.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5g5p.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5gpn.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5grs.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5gsy.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5h7i.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5hnw.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5hnx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5hny.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5i1m.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5iy8.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5iy9.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5iya.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5j4z.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5j7y.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5j8k.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5jb3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5jbh.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5jm0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5jpq.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5k0y.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5k1h.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kbt.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kbu.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kem.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5khr.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kk2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5kne.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5l9t.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ldx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5lmp.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5lms.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ln3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5lqx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5m50.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5mdx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5mpb.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5mqf.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5n5y.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5n5z.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5n60.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5n61.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nd2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nd3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nd7.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5no3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5np0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5np1.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nrl.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nss.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5oam.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ocu.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5oej.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5oqm.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5t4o.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5tzs.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5u05.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5u1f.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5up2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5uz4.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vft.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vh9.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhf.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhh.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhi.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhn.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhp.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vhr.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5viy.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vov.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vvr.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5vvs.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5w9n.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5wcb.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5wen.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5wvi.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5y3r.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5y5z.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ydz.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ye2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ywb.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5z56.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5zam.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5zfu.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a5t.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6acg.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ah0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ahf.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6awc.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6b5b.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6b7z.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6bf7.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6bjs.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6bu9.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6c05.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6c06.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6c3p.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ca0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6d80.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6dbl.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6dqz.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ed3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ejf.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6emk.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6eny.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6f38.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6f42.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6fik.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6fvv.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6g2i.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6gyk.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6gym.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6h58.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hcq.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hiv.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hms.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hqa.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6i27.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6i7o.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6irf.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6j4w.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6jma.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6k9k.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6kw3.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6kw4.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6mj2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6mmm.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6mmt.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6myx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n1q.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n7g.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n7k.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6n8t.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6nme.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6nr8.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6nra.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6olj.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6pas.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ptn.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6pto.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6pvo.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6pwv.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6q0t.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6qc9.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6r7i.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6r7n.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6rkw.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6rxx.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6sb2.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6uby.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6uc0.pdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6upl.pdb </t>
+  </si>
+  <si>
+    <t>Contains DNA and too many chains</t>
+  </si>
+  <si>
+    <t>13 chains, contains MSE residue, needs mutation</t>
+  </si>
+  <si>
+    <t>18 chains similar to 5n5z.pdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains DNA </t>
+  </si>
+  <si>
+    <t>too many chains</t>
+  </si>
+  <si>
+    <t>10 chains</t>
+  </si>
+  <si>
+    <t>8 chains</t>
+  </si>
+  <si>
+    <t>6 chains, contains ATP</t>
+  </si>
+  <si>
+    <t>4 chains</t>
+  </si>
+  <si>
+    <t>16 chains contains multiple sugars</t>
+  </si>
+  <si>
+    <t>6 chains, contains PHOSPHOTHIOPHOSPHORIC ACID-ADENYLATE ESTER</t>
+  </si>
+  <si>
+    <t>13 chains</t>
+  </si>
+  <si>
+    <t>6 chains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 chains, contains sugars (NAG), and UNK peptide </t>
+  </si>
+  <si>
+    <t>8 chains contains ADP</t>
+  </si>
+  <si>
+    <t>no backbone</t>
+  </si>
+  <si>
+    <t>3 chains, contains GDP, GTPm ANP, and taxol</t>
+  </si>
+  <si>
+    <t>12 chains</t>
+  </si>
+  <si>
+    <t>3 chains, contains GDP, GTPm ANP, and taxol similar to 5hny</t>
+  </si>
+  <si>
+    <t>7 chains</t>
+  </si>
+  <si>
+    <t>8 chains contains aATP and ADP</t>
+  </si>
+  <si>
+    <t>similar to 5hny</t>
+  </si>
+  <si>
+    <t>5 chains contains multiple sugars</t>
+  </si>
+  <si>
+    <t>6 chains containa lipid, sugars and ligand</t>
+  </si>
+  <si>
+    <t>similar to 6n7g</t>
+  </si>
+  <si>
+    <t>6 chains, contains ADP</t>
+  </si>
+  <si>
+    <t>4 chains, contains N-ACETYL-D-GLUCOSAMINE (NAG)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1055,8 +2418,22 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1248,6 +2625,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1374,7 +2757,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1417,8 +2800,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1427,8 +2811,11 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1462,6 +2849,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1486,11 +2874,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="2" xr16:uid="{DEC0D320-18C7-404B-BFD2-50D03D5167B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="3" xr16:uid="{0E33F447-600B-1E41-A97E-65A4CE6AA413}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1792,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2691,19 +4083,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203E3033-B15E-BD4D-9992-052B94783655}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>247</v>
       </c>
@@ -2711,7 +4105,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -2728,7 +4122,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -2742,10 +4136,10 @@
         <v>257</v>
       </c>
       <c r="F3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -2758,8 +4152,11 @@
       <c r="E4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -2773,10 +4170,10 @@
         <v>257</v>
       </c>
       <c r="F5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>218</v>
       </c>
@@ -2790,10 +4187,13 @@
         <v>257</v>
       </c>
       <c r="F6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+      <c r="G6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -2806,8 +4206,11 @@
       <c r="E7">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>220</v>
       </c>
@@ -2820,8 +4223,11 @@
       <c r="E8">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>221</v>
       </c>
@@ -2834,8 +4240,11 @@
       <c r="E9">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>222</v>
       </c>
@@ -2848,8 +4257,11 @@
       <c r="E10">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>223</v>
       </c>
@@ -2862,8 +4274,11 @@
       <c r="E11">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -2876,8 +4291,11 @@
       <c r="E12">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -2891,7 +4309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>226</v>
       </c>
@@ -2905,7 +4323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>227</v>
       </c>
@@ -2919,7 +4337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>228</v>
       </c>
@@ -3213,7 +4631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BD96BF-793B-A745-BB28-CF2269D68674}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -3616,4 +5034,3046 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7745B40B-F81E-7347-AA37-59DB198D8F7E}">
+  <dimension ref="A1:O177"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" t="s">
+        <v>540</v>
+      </c>
+      <c r="F1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
+        <v>561</v>
+      </c>
+      <c r="F2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M2" t="s">
+        <v>703</v>
+      </c>
+      <c r="N2">
+        <v>275</v>
+      </c>
+      <c r="O2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="s">
+        <v>569</v>
+      </c>
+      <c r="F3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" t="s">
+        <v>598</v>
+      </c>
+      <c r="N3">
+        <v>236</v>
+      </c>
+      <c r="O3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" t="s">
+        <v>570</v>
+      </c>
+      <c r="F4" t="s">
+        <v>257</v>
+      </c>
+      <c r="M4" t="s">
+        <v>704</v>
+      </c>
+      <c r="N4">
+        <v>160</v>
+      </c>
+      <c r="O4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" t="s">
+        <v>571</v>
+      </c>
+      <c r="F5" t="s">
+        <v>257</v>
+      </c>
+      <c r="M5" t="s">
+        <v>688</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" t="s">
+        <v>572</v>
+      </c>
+      <c r="F6" t="s">
+        <v>257</v>
+      </c>
+      <c r="M6" t="s">
+        <v>691</v>
+      </c>
+      <c r="N6">
+        <v>86</v>
+      </c>
+      <c r="O6" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" t="s">
+        <v>573</v>
+      </c>
+      <c r="F7" t="s">
+        <v>257</v>
+      </c>
+      <c r="M7" t="s">
+        <v>678</v>
+      </c>
+      <c r="N7">
+        <v>38</v>
+      </c>
+      <c r="O7" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>574</v>
+      </c>
+      <c r="F8" t="s">
+        <v>257</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="N8">
+        <v>37</v>
+      </c>
+      <c r="O8" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" t="s">
+        <v>589</v>
+      </c>
+      <c r="F9" t="s">
+        <v>257</v>
+      </c>
+      <c r="M9" t="s">
+        <v>646</v>
+      </c>
+      <c r="N9">
+        <v>34</v>
+      </c>
+      <c r="O9" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" t="s">
+        <v>590</v>
+      </c>
+      <c r="F10" t="s">
+        <v>257</v>
+      </c>
+      <c r="M10" t="s">
+        <v>539</v>
+      </c>
+      <c r="N10">
+        <v>33</v>
+      </c>
+      <c r="O10" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" t="s">
+        <v>593</v>
+      </c>
+      <c r="F11" t="s">
+        <v>257</v>
+      </c>
+      <c r="M11" t="s">
+        <v>617</v>
+      </c>
+      <c r="N11">
+        <v>32</v>
+      </c>
+      <c r="O11" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E12" t="s">
+        <v>264</v>
+      </c>
+      <c r="F12" t="s">
+        <v>257</v>
+      </c>
+      <c r="M12" t="s">
+        <v>709</v>
+      </c>
+      <c r="N12">
+        <v>27</v>
+      </c>
+      <c r="O12" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E13" t="s">
+        <v>594</v>
+      </c>
+      <c r="F13" t="s">
+        <v>257</v>
+      </c>
+      <c r="M13" t="s">
+        <v>567</v>
+      </c>
+      <c r="N13">
+        <v>20</v>
+      </c>
+      <c r="O13" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E14" t="s">
+        <v>595</v>
+      </c>
+      <c r="F14" t="s">
+        <v>257</v>
+      </c>
+      <c r="M14" t="s">
+        <v>562</v>
+      </c>
+      <c r="N14">
+        <v>19</v>
+      </c>
+      <c r="O14" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" t="s">
+        <v>597</v>
+      </c>
+      <c r="F15" t="s">
+        <v>257</v>
+      </c>
+      <c r="M15" t="s">
+        <v>632</v>
+      </c>
+      <c r="N15">
+        <v>19</v>
+      </c>
+      <c r="O15" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>322</v>
+      </c>
+      <c r="E16" t="s">
+        <v>600</v>
+      </c>
+      <c r="F16" t="s">
+        <v>257</v>
+      </c>
+      <c r="M16" t="s">
+        <v>644</v>
+      </c>
+      <c r="N16">
+        <v>18</v>
+      </c>
+      <c r="O16" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" t="s">
+        <v>324</v>
+      </c>
+      <c r="E17" t="s">
+        <v>603</v>
+      </c>
+      <c r="F17" t="s">
+        <v>257</v>
+      </c>
+      <c r="M17" t="s">
+        <v>559</v>
+      </c>
+      <c r="N17">
+        <v>17</v>
+      </c>
+      <c r="O17" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" t="s">
+        <v>604</v>
+      </c>
+      <c r="F18" t="s">
+        <v>257</v>
+      </c>
+      <c r="M18" t="s">
+        <v>653</v>
+      </c>
+      <c r="N18">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B19" t="s">
+        <v>327</v>
+      </c>
+      <c r="E19" t="s">
+        <v>607</v>
+      </c>
+      <c r="F19" t="s">
+        <v>257</v>
+      </c>
+      <c r="M19" t="s">
+        <v>655</v>
+      </c>
+      <c r="N19">
+        <v>15</v>
+      </c>
+      <c r="O19" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B20" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" t="s">
+        <v>629</v>
+      </c>
+      <c r="F20" t="s">
+        <v>257</v>
+      </c>
+      <c r="M20" t="s">
+        <v>663</v>
+      </c>
+      <c r="N20">
+        <v>14</v>
+      </c>
+      <c r="O20" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" t="s">
+        <v>330</v>
+      </c>
+      <c r="E21" t="s">
+        <v>630</v>
+      </c>
+      <c r="F21" t="s">
+        <v>257</v>
+      </c>
+      <c r="M21" t="s">
+        <v>689</v>
+      </c>
+      <c r="N21">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>634</v>
+      </c>
+      <c r="F22" t="s">
+        <v>257</v>
+      </c>
+      <c r="M22" t="s">
+        <v>538</v>
+      </c>
+      <c r="N22">
+        <v>13</v>
+      </c>
+      <c r="O22" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="B23" t="s">
+        <v>333</v>
+      </c>
+      <c r="E23" t="s">
+        <v>640</v>
+      </c>
+      <c r="F23" t="s">
+        <v>257</v>
+      </c>
+      <c r="M23" t="s">
+        <v>686</v>
+      </c>
+      <c r="N23">
+        <v>11</v>
+      </c>
+      <c r="O23" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" t="s">
+        <v>324</v>
+      </c>
+      <c r="E24" t="s">
+        <v>643</v>
+      </c>
+      <c r="F24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" t="s">
+        <v>336</v>
+      </c>
+      <c r="E25" t="s">
+        <v>647</v>
+      </c>
+      <c r="F25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B26" t="s">
+        <v>336</v>
+      </c>
+      <c r="E26" t="s">
+        <v>651</v>
+      </c>
+      <c r="F26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" t="s">
+        <v>654</v>
+      </c>
+      <c r="F27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B28" t="s">
+        <v>341</v>
+      </c>
+      <c r="E28" t="s">
+        <v>659</v>
+      </c>
+      <c r="F28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B29" t="s">
+        <v>327</v>
+      </c>
+      <c r="E29" t="s">
+        <v>667</v>
+      </c>
+      <c r="F29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B30" t="s">
+        <v>344</v>
+      </c>
+      <c r="E30" t="s">
+        <v>668</v>
+      </c>
+      <c r="F30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B31" t="s">
+        <v>306</v>
+      </c>
+      <c r="E31" t="s">
+        <v>671</v>
+      </c>
+      <c r="F31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B32" t="s">
+        <v>330</v>
+      </c>
+      <c r="E32" t="s">
+        <v>672</v>
+      </c>
+      <c r="F32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" t="s">
+        <v>306</v>
+      </c>
+      <c r="E33" t="s">
+        <v>673</v>
+      </c>
+      <c r="F33" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" t="s">
+        <v>349</v>
+      </c>
+      <c r="E34" t="s">
+        <v>677</v>
+      </c>
+      <c r="F34" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E35" t="s">
+        <v>679</v>
+      </c>
+      <c r="F35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B36" t="s">
+        <v>341</v>
+      </c>
+      <c r="E36" t="s">
+        <v>692</v>
+      </c>
+      <c r="F36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B37" t="s">
+        <v>353</v>
+      </c>
+      <c r="E37" t="s">
+        <v>698</v>
+      </c>
+      <c r="F37" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B38" t="s">
+        <v>355</v>
+      </c>
+      <c r="E38" t="s">
+        <v>702</v>
+      </c>
+      <c r="F38" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B39" t="s">
+        <v>357</v>
+      </c>
+      <c r="E39" t="s">
+        <v>706</v>
+      </c>
+      <c r="F39" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" t="s">
+        <v>327</v>
+      </c>
+      <c r="E40" t="s">
+        <v>708</v>
+      </c>
+      <c r="F40" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="B41" t="s">
+        <v>320</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="F41">
+        <v>619</v>
+      </c>
+      <c r="G41" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" t="s">
+        <v>324</v>
+      </c>
+      <c r="E42" t="s">
+        <v>703</v>
+      </c>
+      <c r="F42">
+        <v>275</v>
+      </c>
+      <c r="G42" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B43" t="s">
+        <v>306</v>
+      </c>
+      <c r="E43" t="s">
+        <v>598</v>
+      </c>
+      <c r="F43">
+        <v>236</v>
+      </c>
+      <c r="G43" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B44" t="s">
+        <v>341</v>
+      </c>
+      <c r="E44" t="s">
+        <v>599</v>
+      </c>
+      <c r="F44">
+        <v>221</v>
+      </c>
+      <c r="G44" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B45" t="s">
+        <v>364</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="F45">
+        <v>213</v>
+      </c>
+      <c r="G45" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B46" t="s">
+        <v>315</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>683</v>
+      </c>
+      <c r="F46">
+        <v>200</v>
+      </c>
+      <c r="G46" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B47" t="s">
+        <v>339</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="F47">
+        <v>195</v>
+      </c>
+      <c r="G47" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B48" t="s">
+        <v>368</v>
+      </c>
+      <c r="E48" t="s">
+        <v>704</v>
+      </c>
+      <c r="F48">
+        <v>160</v>
+      </c>
+      <c r="G48" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B49" t="s">
+        <v>368</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="F49">
+        <v>120</v>
+      </c>
+      <c r="G49" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="F50">
+        <v>107</v>
+      </c>
+      <c r="G50" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B51" t="s">
+        <v>372</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="F51">
+        <v>107</v>
+      </c>
+      <c r="G51" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>688</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F53">
+        <v>93</v>
+      </c>
+      <c r="G53" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>691</v>
+      </c>
+      <c r="F54">
+        <v>86</v>
+      </c>
+      <c r="G54" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B55" t="s">
+        <v>322</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="F55">
+        <v>85</v>
+      </c>
+      <c r="G55" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B56" t="s">
+        <v>378</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="F56">
+        <v>75</v>
+      </c>
+      <c r="G56" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B57" t="s">
+        <v>380</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="F57">
+        <v>72</v>
+      </c>
+      <c r="G57" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B58" t="s">
+        <v>341</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="F58">
+        <v>68</v>
+      </c>
+      <c r="G58" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B59" t="s">
+        <v>320</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="F59">
+        <v>63</v>
+      </c>
+      <c r="G59" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B60" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="F60">
+        <v>49</v>
+      </c>
+      <c r="G60" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" t="s">
+        <v>385</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="F61">
+        <v>49</v>
+      </c>
+      <c r="G61" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B62" t="s">
+        <v>385</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="F62">
+        <v>41</v>
+      </c>
+      <c r="G62" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B63" t="s">
+        <v>327</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="F63">
+        <v>40</v>
+      </c>
+      <c r="G63" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B64" t="s">
+        <v>389</v>
+      </c>
+      <c r="E64" t="s">
+        <v>678</v>
+      </c>
+      <c r="F64">
+        <v>38</v>
+      </c>
+      <c r="G64" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B65" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="F65">
+        <v>37</v>
+      </c>
+      <c r="G65" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>391</v>
+      </c>
+      <c r="B66" t="s">
+        <v>392</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="F66">
+        <v>37</v>
+      </c>
+      <c r="G66" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B67" t="s">
+        <v>341</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="F67">
+        <v>36</v>
+      </c>
+      <c r="G67" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B68" t="s">
+        <v>213</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="F68">
+        <v>36</v>
+      </c>
+      <c r="G68" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B69" t="s">
+        <v>341</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="F69">
+        <v>34</v>
+      </c>
+      <c r="G69" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B70" t="s">
+        <v>324</v>
+      </c>
+      <c r="E70" t="s">
+        <v>646</v>
+      </c>
+      <c r="F70">
+        <v>34</v>
+      </c>
+      <c r="G70" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B71" t="s">
+        <v>336</v>
+      </c>
+      <c r="E71" t="s">
+        <v>539</v>
+      </c>
+      <c r="F71">
+        <v>33</v>
+      </c>
+      <c r="G71" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="F72">
+        <v>33</v>
+      </c>
+      <c r="G72" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E73" t="s">
+        <v>617</v>
+      </c>
+      <c r="F73">
+        <v>32</v>
+      </c>
+      <c r="G73" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="F74">
+        <v>31</v>
+      </c>
+      <c r="G74" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E75" t="s">
+        <v>709</v>
+      </c>
+      <c r="F75">
+        <v>27</v>
+      </c>
+      <c r="G75" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="F76">
+        <v>25</v>
+      </c>
+      <c r="G76" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="F77">
+        <v>25</v>
+      </c>
+      <c r="G77" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="F78">
+        <v>24</v>
+      </c>
+      <c r="G78" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="F79">
+        <v>24</v>
+      </c>
+      <c r="G79" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E80" t="s">
+        <v>567</v>
+      </c>
+      <c r="F80">
+        <v>20</v>
+      </c>
+      <c r="G80" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E81" t="s">
+        <v>562</v>
+      </c>
+      <c r="F81">
+        <v>19</v>
+      </c>
+      <c r="G81" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E82" t="s">
+        <v>632</v>
+      </c>
+      <c r="F82">
+        <v>19</v>
+      </c>
+      <c r="G82" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="F83">
+        <v>19</v>
+      </c>
+      <c r="G83" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F84">
+        <v>19</v>
+      </c>
+      <c r="G84" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="F85">
+        <v>18</v>
+      </c>
+      <c r="G85" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E86" t="s">
+        <v>644</v>
+      </c>
+      <c r="F86">
+        <v>18</v>
+      </c>
+      <c r="G86" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="E87" t="s">
+        <v>559</v>
+      </c>
+      <c r="F87">
+        <v>17</v>
+      </c>
+      <c r="G87" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E88" t="s">
+        <v>653</v>
+      </c>
+      <c r="F88">
+        <v>15</v>
+      </c>
+      <c r="G88" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E89" t="s">
+        <v>655</v>
+      </c>
+      <c r="F89">
+        <v>15</v>
+      </c>
+      <c r="G89" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="F90">
+        <v>14</v>
+      </c>
+      <c r="G90" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E91" t="s">
+        <v>663</v>
+      </c>
+      <c r="F91">
+        <v>14</v>
+      </c>
+      <c r="G91" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E92" t="s">
+        <v>689</v>
+      </c>
+      <c r="F92">
+        <v>14</v>
+      </c>
+      <c r="G92" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="F93">
+        <v>14</v>
+      </c>
+      <c r="G93" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="F94">
+        <v>14</v>
+      </c>
+      <c r="G94" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E95" t="s">
+        <v>538</v>
+      </c>
+      <c r="F95">
+        <v>13</v>
+      </c>
+      <c r="G95" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="F96">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E97" t="s">
+        <v>686</v>
+      </c>
+      <c r="F97">
+        <v>11</v>
+      </c>
+      <c r="G97" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="F98">
+        <v>10</v>
+      </c>
+      <c r="G98" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E99" t="s">
+        <v>616</v>
+      </c>
+      <c r="F99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E100" t="s">
+        <v>641</v>
+      </c>
+      <c r="F100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="E101" t="s">
+        <v>650</v>
+      </c>
+      <c r="F101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="E102" t="s">
+        <v>553</v>
+      </c>
+      <c r="F102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="E103" t="s">
+        <v>560</v>
+      </c>
+      <c r="F103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E104" t="s">
+        <v>581</v>
+      </c>
+      <c r="F104">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E105" t="s">
+        <v>582</v>
+      </c>
+      <c r="F105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E106" t="s">
+        <v>585</v>
+      </c>
+      <c r="F106">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E107" t="s">
+        <v>657</v>
+      </c>
+      <c r="F107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E108" t="s">
+        <v>685</v>
+      </c>
+      <c r="F108">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E109" t="s">
+        <v>564</v>
+      </c>
+      <c r="F109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E110" t="s">
+        <v>649</v>
+      </c>
+      <c r="F110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E111" t="s">
+        <v>555</v>
+      </c>
+      <c r="F111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E112" t="s">
+        <v>586</v>
+      </c>
+      <c r="F112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E113" t="s">
+        <v>626</v>
+      </c>
+      <c r="F113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="E114" t="s">
+        <v>639</v>
+      </c>
+      <c r="F114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E115" t="s">
+        <v>624</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E116" t="s">
+        <v>625</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E117" t="s">
+        <v>633</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E118" t="s">
+        <v>642</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E119" t="s">
+        <v>648</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="E120" t="s">
+        <v>661</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E121" t="s">
+        <v>707</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="E122" t="s">
+        <v>545</v>
+      </c>
+      <c r="F122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E123" t="s">
+        <v>546</v>
+      </c>
+      <c r="F123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="E124" t="s">
+        <v>556</v>
+      </c>
+      <c r="F124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="E125" t="s">
+        <v>615</v>
+      </c>
+      <c r="F125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E126" t="s">
+        <v>666</v>
+      </c>
+      <c r="F126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="E127" t="s">
+        <v>557</v>
+      </c>
+      <c r="F127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="E128" t="s">
+        <v>592</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="E129" t="s">
+        <v>674</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="E130" t="s">
+        <v>694</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E131" t="s">
+        <v>695</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E132" t="s">
+        <v>699</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E133" t="s">
+        <v>536</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E134" t="s">
+        <v>537</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="E135" t="s">
+        <v>541</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="E136" t="s">
+        <v>542</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E137" t="s">
+        <v>547</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="E138" t="s">
+        <v>548</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E139" t="s">
+        <v>549</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E140" t="s">
+        <v>550</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E141" t="s">
+        <v>551</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="E142" t="s">
+        <v>552</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E143" t="s">
+        <v>554</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E144" t="s">
+        <v>558</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E145" t="s">
+        <v>563</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="E146" t="s">
+        <v>568</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E147" t="s">
+        <v>577</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E148" t="s">
+        <v>579</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E149" t="s">
+        <v>580</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E150" t="s">
+        <v>583</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="E151" t="s">
+        <v>584</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="E152" t="s">
+        <v>587</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E153" t="s">
+        <v>591</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E154" t="s">
+        <v>601</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E155" t="s">
+        <v>602</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E156" t="s">
+        <v>605</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E157" t="s">
+        <v>606</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E158" t="s">
+        <v>609</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E159" t="s">
+        <v>610</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="E160" t="s">
+        <v>611</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="E161" t="s">
+        <v>620</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E162" t="s">
+        <v>628</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="E163" t="s">
+        <v>631</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E164" t="s">
+        <v>636</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E165" t="s">
+        <v>637</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E166" t="s">
+        <v>638</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E167" t="s">
+        <v>652</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E168" t="s">
+        <v>660</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E169" t="s">
+        <v>662</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="E170" t="s">
+        <v>675</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="E171" t="s">
+        <v>676</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E172" t="s">
+        <v>681</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E173" t="s">
+        <v>684</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="B174" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="E174" t="s">
+        <v>687</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E175" t="s">
+        <v>696</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="E176" t="s">
+        <v>701</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="E1:F176">
+    <sortCondition descending="1" ref="F1:F176"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://www.pdbe.org/6uby" xr:uid="{B66B727D-A2F9-194E-B203-99C0FEE1FA5D}"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://www.pdbe.org/6uc0" xr:uid="{D31B9CA2-CDF6-DD4F-AA5A-D2B1D3288B2A}"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://www.pdbe.org/6k9k" xr:uid="{CFA3F2B0-300B-AA45-817B-DC9E0CF24D28}"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://www.pdbe.org/6pwv" xr:uid="{720427F1-649D-704C-9377-4566EEB7F202}"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://www.pdbe.org/6upl" xr:uid="{DE75C579-84E3-D749-A7C9-3C315C84539E}"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://www.pdbe.org/6olj" xr:uid="{22F89526-D9D3-3240-8CEE-D15766548C0C}"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://www.pdbe.org/6pto" xr:uid="{738DB771-D90D-174E-A73B-6DEB57181F28}"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://www.pdbe.org/6kw3" xr:uid="{C613251D-5035-8946-ABD5-3F194B356D7B}"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://www.pdbe.org/6kw4" xr:uid="{1B3D9152-F68E-BF45-82AB-16A603D494BD}"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://www.pdbe.org/6rkw" xr:uid="{B39EE6F3-C9A0-9A44-A9FE-D8E9603A3441}"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://www.pdbe.org/6pas" xr:uid="{E6697BF0-D406-8B41-9A53-1B85ECB1B817}"/>
+    <hyperlink ref="A13" r:id="rId12" display="http://www.pdbe.org/6pvo" xr:uid="{BA508D02-F917-9C49-BBDA-669E142FB328}"/>
+    <hyperlink ref="A14" r:id="rId13" display="http://www.pdbe.org/6sb2" xr:uid="{53488509-A2D9-4248-9FCC-3AEFFC28A946}"/>
+    <hyperlink ref="A15" r:id="rId14" display="http://www.pdbe.org/6q0t" xr:uid="{67FCBDD4-D35E-4A4F-A19A-01C3F4D206DD}"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://www.pdbe.org/6r7i" xr:uid="{AE3924B3-BA38-D240-9030-DCD68C81F4F9}"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://www.pdbe.org/6r7n" xr:uid="{0CCED457-15F7-B94B-AF29-367937755435}"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://www.pdbe.org/6qc9" xr:uid="{46E05CF9-75DE-9441-BE65-ADB459B7D739}"/>
+    <hyperlink ref="A20" r:id="rId18" display="http://www.pdbe.org/6nr8" xr:uid="{04612664-26AD-384B-A610-55E7682991A0}"/>
+    <hyperlink ref="A21" r:id="rId19" display="http://www.pdbe.org/6nra" xr:uid="{BD34CFE1-DB48-D44E-B0C8-F7DA976DC27F}"/>
+    <hyperlink ref="A22" r:id="rId20" display="http://www.pdbe.org/6myx" xr:uid="{E4CFF1CB-8DB0-5E4A-8F25-C18B59D03029}"/>
+    <hyperlink ref="A23" r:id="rId21" display="http://www.pdbe.org/6nme" xr:uid="{ACE60666-A2F6-F54F-9EE3-45F19AD3249A}"/>
+    <hyperlink ref="A24" r:id="rId22" display="http://www.pdbe.org/6n7k" xr:uid="{8DD4D8C2-1630-3840-8194-A4D94ACBF56F}"/>
+    <hyperlink ref="A25" r:id="rId23" display="http://www.pdbe.org/6n7g" xr:uid="{E67FCF8C-FCC2-7C43-92B5-03BCED9CFB01}"/>
+    <hyperlink ref="A26" r:id="rId24" display="http://www.pdbe.org/6jma" xr:uid="{1A8A0383-AB47-B24F-B502-02F1E6F7108B}"/>
+    <hyperlink ref="A27" r:id="rId25" display="http://www.pdbe.org/6j4w" xr:uid="{0247EC85-442E-2945-909B-310ADA376059}"/>
+    <hyperlink ref="A28" r:id="rId26" display="http://www.pdbe.org/6ahf" xr:uid="{435C0D77-C979-134E-8917-91F36B2FB500}"/>
+    <hyperlink ref="A29" r:id="rId27" display="http://www.pdbe.org/6hms" xr:uid="{5DC10912-1C47-E742-AE2A-AF4141F63E07}"/>
+    <hyperlink ref="A30" r:id="rId28" display="http://www.pdbe.org/6i7o" xr:uid="{C894B4BF-EAFB-084E-BB53-88C0741C5B28}"/>
+    <hyperlink ref="A31" r:id="rId29" display="http://www.pdbe.org/6irf" xr:uid="{3D907D48-D686-8941-8E4E-8DB21C61FEB0}"/>
+    <hyperlink ref="A32" r:id="rId30" display="http://www.pdbe.org/6n8t" xr:uid="{D3089E86-515D-D842-9956-4E80BDF85B62}"/>
+    <hyperlink ref="A33" r:id="rId31" display="http://www.pdbe.org/6i27" xr:uid="{7E0538AA-8643-FC4A-A259-0AEA1F2613CE}"/>
+    <hyperlink ref="A34" r:id="rId32" display="http://www.pdbe.org/6mj2" xr:uid="{49B78346-AB3A-5849-B3FF-C3A1B9A9337E}"/>
+    <hyperlink ref="A35" r:id="rId33" display="http://www.pdbe.org/6gyk" xr:uid="{066708ED-C67D-C745-A8FE-975E567AFA1D}"/>
+    <hyperlink ref="A36" r:id="rId34" display="http://www.pdbe.org/6gym" xr:uid="{895C5269-1D6D-EC41-A809-E7F0940CEC6B}"/>
+    <hyperlink ref="A37" r:id="rId35" display="http://www.pdbe.org/6n1q" xr:uid="{507D15F1-EFD3-D346-895B-76510BB1661B}"/>
+    <hyperlink ref="A38" r:id="rId36" display="http://www.pdbe.org/6mmm" xr:uid="{7B1D9595-8778-334D-8D2F-2BCCFCCB3A24}"/>
+    <hyperlink ref="A39" r:id="rId37" display="http://www.pdbe.org/6mmt" xr:uid="{C3AB8EAF-44E9-4347-BEF2-D1249095CE18}"/>
+    <hyperlink ref="A40" r:id="rId38" display="http://www.pdbe.org/6hqa" xr:uid="{AA8C5E1E-9A15-F341-9B74-8A22A5273AB9}"/>
+    <hyperlink ref="A41" r:id="rId39" display="http://www.pdbe.org/6ah0" xr:uid="{99CBD472-0829-9945-9F9A-F75A436CEBBB}"/>
+    <hyperlink ref="A42" r:id="rId40" display="http://www.pdbe.org/6hcq" xr:uid="{108ABE37-C0C6-B34C-A4A0-36B773669939}"/>
+    <hyperlink ref="A43" r:id="rId41" display="http://www.pdbe.org/6hiv" xr:uid="{EEB07AE6-C740-A24D-820C-7B9E599B5274}"/>
+    <hyperlink ref="A44" r:id="rId42" display="http://www.pdbe.org/6a5t" xr:uid="{0DCB17DB-D512-9943-81BD-F7D50FAA06CA}"/>
+    <hyperlink ref="A45" r:id="rId43" display="http://www.pdbe.org/6ed3" xr:uid="{090C6A79-F1EF-5B44-A4EA-7062395E1706}"/>
+    <hyperlink ref="A46" r:id="rId44" display="http://www.pdbe.org/5z56" xr:uid="{0ABE88C4-2FCA-AF45-972E-CA64F6E2EB6D}"/>
+    <hyperlink ref="A47" r:id="rId45" display="http://www.pdbe.org/6h58" xr:uid="{5C6B4EB8-567C-414D-8283-36CA53E46163}"/>
+    <hyperlink ref="A48" r:id="rId46" display="http://www.pdbe.org/6fvv" xr:uid="{563DAA6F-7E73-7646-BD80-70EB80EF3CC8}"/>
+    <hyperlink ref="A49" r:id="rId47" display="http://www.pdbe.org/6acg" xr:uid="{F6C23545-65B2-4049-B6FB-2D6A6AB3C0DA}"/>
+    <hyperlink ref="A50" r:id="rId48" display="http://www.pdbe.org/6ejf" xr:uid="{F5160351-B5CD-FB40-BBB6-CF32AFA6DE7F}"/>
+    <hyperlink ref="A51" r:id="rId49" display="http://www.pdbe.org/6dqz" xr:uid="{C07287E1-E4F6-2248-BE64-F2B1B2C9A946}"/>
+    <hyperlink ref="A52" r:id="rId50" display="http://www.pdbe.org/6dbl" xr:uid="{2AD99896-B60F-5D4D-B208-44B0E7333F90}"/>
+    <hyperlink ref="A53" r:id="rId51" display="http://www.pdbe.org/5vft" xr:uid="{A94AE766-87ED-E349-8574-72FF64920879}"/>
+    <hyperlink ref="A54" r:id="rId52" display="http://www.pdbe.org/6d80" xr:uid="{A4379BA6-F265-B748-87F5-882F14B3B8C8}"/>
+    <hyperlink ref="A55" r:id="rId53" display="http://www.pdbe.org/6g2i" xr:uid="{EE847ACF-5C7A-AB42-91F7-6D0DDC023834}"/>
+    <hyperlink ref="A56" r:id="rId54" display="http://www.pdbe.org/5ywb" xr:uid="{047EA4F7-BD4E-E54A-BC03-D1CB7F8E218F}"/>
+    <hyperlink ref="A57" r:id="rId55" display="http://www.pdbe.org/5oqm" xr:uid="{3AC34462-3F1F-FA48-8145-07715581FA6E}"/>
+    <hyperlink ref="A58" r:id="rId56" display="http://www.pdbe.org/5zfu" xr:uid="{3392F600-0489-CE4B-99FB-164DE021DC45}"/>
+    <hyperlink ref="A59" r:id="rId57" display="http://www.pdbe.org/5zam" xr:uid="{4E63CAFB-F4D8-4143-9EC9-0BD182353853}"/>
+    <hyperlink ref="A60" r:id="rId58" display="http://www.pdbe.org/6bjs" xr:uid="{4DA0B663-4BB7-C94A-9212-6C7CB809B44F}"/>
+    <hyperlink ref="A61" r:id="rId59" display="http://www.pdbe.org/6c05" xr:uid="{86CEC2B1-684B-564D-A972-2D71FD84F5CF}"/>
+    <hyperlink ref="A62" r:id="rId60" display="http://www.pdbe.org/6c06" xr:uid="{CCF797D5-C806-7044-AC16-A50AC794DCE9}"/>
+    <hyperlink ref="A63" r:id="rId61" display="http://www.pdbe.org/6fik" xr:uid="{DA979DB3-3250-0047-AC6B-BC855F812E3C}"/>
+    <hyperlink ref="A64" r:id="rId62" display="http://www.pdbe.org/6ca0" xr:uid="{51F6E530-7EE6-CA45-A9AB-3436B0F42B39}"/>
+    <hyperlink ref="A65" r:id="rId63" display="http://www.pdbe.org/6bf7" xr:uid="{23B8ABC8-BE1D-A545-B444-0A57274B7AA9}"/>
+    <hyperlink ref="A67" r:id="rId64" display="http://www.pdbe.org/6f38" xr:uid="{82D50D36-7DAF-FA4D-AFCC-7949A6FF2DB0}"/>
+    <hyperlink ref="A68" r:id="rId65" display="http://www.pdbe.org/6f42" xr:uid="{982C7234-DAFF-A643-BEE5-29FE30FA9787}"/>
+    <hyperlink ref="A69" r:id="rId66" display="http://www.pdbe.org/5y5z" xr:uid="{E6226081-7F00-7A4F-8AC6-5B0EE745D103}"/>
+    <hyperlink ref="A70" r:id="rId67" display="http://www.pdbe.org/6b7z" xr:uid="{53025468-48DB-6F4A-99AB-04AAFC7C2FDA}"/>
+    <hyperlink ref="A71" r:id="rId68" display="http://www.pdbe.org/6bu9" xr:uid="{C60583D0-0F5D-6142-B413-7C25C5899334}"/>
+    <hyperlink ref="A72" r:id="rId69" display="http://www.pdbe.org/5ydz" xr:uid="{FD9200CB-7717-C943-883D-1300A944AD34}"/>
+    <hyperlink ref="A73" r:id="rId70" display="http://www.pdbe.org/5ye2" xr:uid="{79597C9A-EB89-854F-BB97-87B927D04045}"/>
+    <hyperlink ref="A74" r:id="rId71" display="http://www.pdbe.org/6emk" xr:uid="{39F58F19-B4A5-E047-A1E5-1F6E3BEAA480}"/>
+    <hyperlink ref="A75" r:id="rId72" display="http://www.pdbe.org/6eny" xr:uid="{167675A3-2235-BD47-814F-3A304B982037}"/>
+    <hyperlink ref="A76" r:id="rId73" display="http://www.pdbe.org/5vvr" xr:uid="{5D395E14-B07C-434C-81B0-B3F63B4D3614}"/>
+    <hyperlink ref="A77" r:id="rId74" display="http://www.pdbe.org/5vvs" xr:uid="{D2F0B7C9-384C-794F-BD14-BB3869C40D23}"/>
+    <hyperlink ref="A78" r:id="rId75" display="http://www.pdbe.org/6b5b" xr:uid="{D0FB7DD0-8EE0-D047-A1C9-C5665C869C11}"/>
+    <hyperlink ref="A79" r:id="rId76" display="http://www.pdbe.org/5oam" xr:uid="{6D0E1F33-B837-4F41-988E-E9D21CF58F70}"/>
+    <hyperlink ref="A80" r:id="rId77" display="http://www.pdbe.org/5ocu" xr:uid="{A95EF330-7968-8D4A-B74E-26F04903AC68}"/>
+    <hyperlink ref="A81" r:id="rId78" display="http://www.pdbe.org/6awc" xr:uid="{A90EF799-D2A0-B043-A205-29EF88690BEB}"/>
+    <hyperlink ref="A82" r:id="rId79" display="http://www.pdbe.org/5m50" xr:uid="{8C7F7EC1-6888-5D4D-9F1C-21D278C9A350}"/>
+    <hyperlink ref="A83" r:id="rId80" display="http://www.pdbe.org/5m54" xr:uid="{DF462713-92DF-9D43-B16C-A342203588D8}"/>
+    <hyperlink ref="A84" r:id="rId81" display="http://www.pdbe.org/5nd2" xr:uid="{7A6194B4-6AD5-B640-AF98-F79F6B64875F}"/>
+    <hyperlink ref="A85" r:id="rId82" display="http://www.pdbe.org/5nd3" xr:uid="{5C7B4692-673E-FD46-A371-64612EF9C570}"/>
+    <hyperlink ref="A86" r:id="rId83" display="http://www.pdbe.org/5nd7" xr:uid="{F3E16601-F55F-EC4A-BED6-0A29D3C280C3}"/>
+    <hyperlink ref="A87" r:id="rId84" display="http://www.pdbe.org/5y3r" xr:uid="{C588B26E-4F0E-6C41-A212-6FA897DFA5D6}"/>
+    <hyperlink ref="A88" r:id="rId85" display="http://www.pdbe.org/5vh9" xr:uid="{13A7DE40-0222-304B-B1D3-5990825C003C}"/>
+    <hyperlink ref="A89" r:id="rId86" display="http://www.pdbe.org/5vhn" xr:uid="{6FE10AEF-41A6-A04F-B91C-2456BA688C9E}"/>
+    <hyperlink ref="A90" r:id="rId87" display="http://www.pdbe.org/5vhp" xr:uid="{9E90FEC7-C522-9B44-985B-903DF9925971}"/>
+    <hyperlink ref="A91" r:id="rId88" display="http://www.pdbe.org/5vhr" xr:uid="{0A9F47BC-DDAD-CD43-90F0-E60654CA454B}"/>
+    <hyperlink ref="A92" r:id="rId89" display="http://www.pdbe.org/5vhf" xr:uid="{58A05D82-A020-AF4B-9AEE-B2A624138EAD}"/>
+    <hyperlink ref="A93" r:id="rId90" display="http://www.pdbe.org/5vhh" xr:uid="{70CC51A9-B633-B548-BD8A-65B3AF6C9731}"/>
+    <hyperlink ref="A94" r:id="rId91" display="http://www.pdbe.org/5vhi" xr:uid="{18242348-1EFD-C44C-95F4-DFCD562866B3}"/>
+    <hyperlink ref="A95" r:id="rId92" display="http://www.pdbe.org/5w9n" xr:uid="{5549C629-B7AF-9D45-85B2-E70265C63A6B}"/>
+    <hyperlink ref="A96" r:id="rId93" display="http://www.pdbe.org/5wcb" xr:uid="{4DA840D0-FE0E-324F-9E28-CDBD0C6AF968}"/>
+    <hyperlink ref="A97" r:id="rId94" display="http://www.pdbe.org/5oej" xr:uid="{A5B56F87-5E72-8E49-B21B-7BFB700B0FDD}"/>
+    <hyperlink ref="A98" r:id="rId95" display="http://www.pdbe.org/5wen" xr:uid="{2507006D-D2D7-C147-AD7E-401E81B8290A}"/>
+    <hyperlink ref="A99" r:id="rId96" display="http://www.pdbe.org/5nss" xr:uid="{B7D1CAAA-0954-594B-B8C3-E26A45A8B276}"/>
+    <hyperlink ref="A100" r:id="rId97" display="http://www.pdbe.org/5mdx" xr:uid="{E393635A-1557-0540-A4DE-21EFCAECD747}"/>
+    <hyperlink ref="A101" r:id="rId98" display="http://www.pdbe.org/5viy" xr:uid="{73EE12AA-A97C-A14E-B0B7-81FE41B843D3}"/>
+    <hyperlink ref="A102" r:id="rId99" display="http://www.pdbe.org/5no3" xr:uid="{1C3D5AC7-857E-8C4B-9E9D-3194B01DEBF0}"/>
+    <hyperlink ref="A103" r:id="rId100" display="http://www.pdbe.org/5nrl" xr:uid="{3D20CB62-C571-D543-8775-24960DD9C249}"/>
+    <hyperlink ref="A104" r:id="rId101" display="http://www.pdbe.org/5np0" xr:uid="{2237CBB8-A182-2C4E-BD5E-46AE3E797028}"/>
+    <hyperlink ref="A105" r:id="rId102" display="http://www.pdbe.org/5np1" xr:uid="{6FEE0C93-236C-424A-ACA5-E679E69921E2}"/>
+    <hyperlink ref="A106" r:id="rId103" display="http://www.pdbe.org/5u05" xr:uid="{64142526-39B2-B045-93D3-2FE621363C41}"/>
+    <hyperlink ref="A107" r:id="rId104" display="http://www.pdbe.org/5uz4" xr:uid="{FFFD51A6-A800-844A-AE47-1913169E74A4}"/>
+    <hyperlink ref="A108" r:id="rId105" display="http://www.pdbe.org/5n61" xr:uid="{27EBD349-F47D-0B4B-8124-E87DA444C313}"/>
+    <hyperlink ref="A109" r:id="rId106" display="http://www.pdbe.org/5gpn" xr:uid="{AB370129-B4FD-414E-9DD4-BE00E12DCDAD}"/>
+    <hyperlink ref="A110" r:id="rId107" display="http://www.pdbe.org/5n60" xr:uid="{9DFC7DEB-262C-954B-A697-913979CF4E43}"/>
+    <hyperlink ref="A111" r:id="rId108" display="http://www.pdbe.org/5n5z" xr:uid="{6EA89DC3-5BD1-154E-94E4-DE37D4A4EE6F}"/>
+    <hyperlink ref="A112" r:id="rId109" display="http://www.pdbe.org/5n5y" xr:uid="{3034336C-921F-B647-8C2C-EC3ADB43123B}"/>
+    <hyperlink ref="A113" r:id="rId110" display="http://www.pdbe.org/5ln3" xr:uid="{C23ECDFD-7D30-7744-9590-507FC4A0714B}"/>
+    <hyperlink ref="A114" r:id="rId111" display="http://www.pdbe.org/5mqf" xr:uid="{ADF0D0FA-5EBB-0D4B-B3D0-26B8A5907ECD}"/>
+    <hyperlink ref="A115" r:id="rId112" display="http://www.pdbe.org/5wvi" xr:uid="{5D99405C-7C8D-6547-937B-5448F8A509BB}"/>
+    <hyperlink ref="A116" r:id="rId113" display="http://www.pdbe.org/5up2" xr:uid="{576791CE-36A7-C246-A406-2485D3B47693}"/>
+    <hyperlink ref="A117" r:id="rId114" display="http://www.pdbe.org/5mpb" xr:uid="{81F31976-9DB8-304A-BFEB-053ADCDFAF16}"/>
+    <hyperlink ref="A118" r:id="rId115" display="http://www.pdbe.org/6ptn" xr:uid="{27462E35-AC1A-7747-AEC8-E19BBF7F4AFA}"/>
+    <hyperlink ref="A119" r:id="rId116" display="http://www.pdbe.org/5u1f" xr:uid="{4CF163E7-006F-7E49-A55C-E8C89FC62965}"/>
+    <hyperlink ref="A120" r:id="rId117" display="http://www.pdbe.org/5h7i" xr:uid="{20D94FE6-3377-9249-B02C-BB2153244E53}"/>
+    <hyperlink ref="A121" r:id="rId118" display="http://www.pdbe.org/5t4o" xr:uid="{18734EF7-D0FA-144F-9625-11F933F5383B}"/>
+    <hyperlink ref="A122" r:id="rId119" display="http://www.pdbe.org/5tzs" xr:uid="{6933CED1-0F19-FB4F-B52D-8373F04AFAF1}"/>
+    <hyperlink ref="A123" r:id="rId120" display="http://www.pdbe.org/5grs" xr:uid="{D512746D-BC7C-0A45-8536-B14534C9DA21}"/>
+    <hyperlink ref="A124" r:id="rId121" display="http://www.pdbe.org/5jbh" xr:uid="{FBC283DE-E780-9149-8757-B8434EFCA748}"/>
+    <hyperlink ref="A125" r:id="rId122" display="http://www.pdbe.org/5jb3" xr:uid="{AE8938F4-23EF-FF4E-88DD-5F5B0313A045}"/>
+    <hyperlink ref="A126" r:id="rId123" display="http://www.pdbe.org/5lqx" xr:uid="{C99C216E-076B-2B4D-B559-538776C3A569}"/>
+    <hyperlink ref="A127" r:id="rId124" display="http://www.pdbe.org/5lmp" xr:uid="{3DF4A993-7758-0D47-9AEC-1C99C38E35EC}"/>
+    <hyperlink ref="A128" r:id="rId125" display="http://www.pdbe.org/5lms" xr:uid="{1C8B019C-BBFC-6743-949C-1BAC2C02BFD8}"/>
+    <hyperlink ref="A129" r:id="rId126" display="http://www.pdbe.org/5j7y" xr:uid="{6BE6DAE5-79A8-9F4C-BCE6-A543EDF94015}"/>
+    <hyperlink ref="A130" r:id="rId127" display="http://www.pdbe.org/5j8k" xr:uid="{798E13EB-09BD-9C49-B75D-6C235FFF62CA}"/>
+    <hyperlink ref="A131" r:id="rId128" display="http://www.pdbe.org/5j4z" xr:uid="{D3D93BAB-7046-D34C-BF82-2FDCEBB7422F}"/>
+    <hyperlink ref="A132" r:id="rId129" display="http://www.pdbe.org/5gsy" xr:uid="{AF530535-F2C5-0D46-846C-9A9674AF4A0B}"/>
+    <hyperlink ref="A133" r:id="rId130" display="http://www.pdbe.org/5fkx" xr:uid="{BF28C06B-DC37-4B45-93F5-5A48FB38AC1D}"/>
+    <hyperlink ref="A134" r:id="rId131" display="http://www.pdbe.org/5ldx" xr:uid="{BAEC9A8D-5046-DA4E-9085-FD0BC5AC093C}"/>
+    <hyperlink ref="A135" r:id="rId132" display="http://www.pdbe.org/5hnw" xr:uid="{83325A6C-7B75-8F4E-8027-025AD10CCA44}"/>
+    <hyperlink ref="A136" r:id="rId133" display="http://www.pdbe.org/5kem" xr:uid="{549601B9-769D-C545-A4CA-CB6AC141537E}"/>
+    <hyperlink ref="A137" r:id="rId134" display="http://www.pdbe.org/5khr" xr:uid="{41E5933F-F76D-1744-BA7D-E16285B82C4C}"/>
+    <hyperlink ref="A138" r:id="rId135" display="http://www.pdbe.org/5hnx" xr:uid="{BBE79E76-72EE-B24B-A424-0DEEE513D945}"/>
+    <hyperlink ref="A139" r:id="rId136" display="http://www.pdbe.org/5hny" xr:uid="{E82483F2-0401-B348-B1F6-444B6571B406}"/>
+    <hyperlink ref="A140" r:id="rId137" display="http://www.pdbe.org/5jpq" xr:uid="{73075A99-E149-6241-BA20-04DF7FF3A469}"/>
+    <hyperlink ref="A141" r:id="rId138" display="http://www.pdbe.org/5g5p" xr:uid="{1116C442-27E2-CE49-A5DC-6E5F46536F00}"/>
+    <hyperlink ref="A142" r:id="rId139" display="http://www.pdbe.org/5kne" xr:uid="{726217F5-A3CD-6D45-9B14-33DFBA490D76}"/>
+    <hyperlink ref="A143" r:id="rId140" display="http://www.pdbe.org/5l9t" xr:uid="{E15AD173-76C4-B345-8BE8-9AB0FC6C3891}"/>
+    <hyperlink ref="A144" r:id="rId141" display="http://www.pdbe.org/5g4f" xr:uid="{D03C774D-67EA-AD4A-B5F8-3F30B9FFF927}"/>
+    <hyperlink ref="A145" r:id="rId142" display="http://www.pdbe.org/5k0y" xr:uid="{5F01E7A0-E6D9-2F43-A4A1-C2E55D668ACC}"/>
+    <hyperlink ref="A146" r:id="rId143" display="http://www.pdbe.org/5kbt" xr:uid="{FAC0324E-17C4-AE47-B8A9-752D1021F1B9}"/>
+    <hyperlink ref="A147" r:id="rId144" display="http://www.pdbe.org/5kbu" xr:uid="{46E9542C-7AC8-6F4A-8637-3E3C587CB7F4}"/>
+    <hyperlink ref="A148" r:id="rId145" display="http://www.pdbe.org/5k1h" xr:uid="{52B255F8-EC84-F84A-B6A6-0FE53C7E8355}"/>
+    <hyperlink ref="A149" r:id="rId146" display="http://www.pdbe.org/5vov" xr:uid="{5A300447-46EF-F743-86EF-A10271BAF9CB}"/>
+    <hyperlink ref="A150" r:id="rId147" display="http://www.pdbe.org/5kk2" xr:uid="{D567B832-065D-644F-BF68-5566F390E704}"/>
+    <hyperlink ref="A151" r:id="rId148" display="http://www.pdbe.org/5fwp" xr:uid="{3EDF286B-BAB7-4944-8829-4A8AD5E5BD15}"/>
+    <hyperlink ref="A152" r:id="rId149" display="http://www.pdbe.org/5fwm" xr:uid="{EFFF4E59-6125-0E4F-8541-AB122121B5E7}"/>
+    <hyperlink ref="A153" r:id="rId150" display="http://www.pdbe.org/5jm0" xr:uid="{97D8A177-BCC4-094C-98CF-F36BCA1E3D00}"/>
+    <hyperlink ref="A154" r:id="rId151" display="http://www.pdbe.org/5iy9" xr:uid="{D63FABD2-0E38-1543-A44C-BD2FD6DCEA0B}"/>
+    <hyperlink ref="A155" r:id="rId152" display="http://www.pdbe.org/5iy8" xr:uid="{1A3EC254-3984-8446-8C60-EAD68F77B211}"/>
+    <hyperlink ref="A156" r:id="rId153" display="http://www.pdbe.org/5iya" xr:uid="{F6C83053-F224-3F48-A94E-54CEC0BCA992}"/>
+    <hyperlink ref="A157" r:id="rId154" display="http://www.pdbe.org/5fxh" xr:uid="{1DEF6E56-B3E9-3543-8DFA-D9ADD1287B42}"/>
+    <hyperlink ref="A158" r:id="rId155" display="http://www.pdbe.org/3jcr" xr:uid="{2E849754-9FF7-6745-961C-1D69EB39F1DB}"/>
+    <hyperlink ref="A159" r:id="rId156" display="http://www.pdbe.org/5i1m" xr:uid="{A1B733D6-986A-4044-9036-9CC6594BB3FC}"/>
+    <hyperlink ref="A160" r:id="rId157" display="http://www.pdbe.org/3jcg" xr:uid="{4548096D-CEAD-334F-94DF-CBF9F29BCFFF}"/>
+    <hyperlink ref="A161" r:id="rId158" display="http://www.pdbe.org/3jch" xr:uid="{62F5111F-F4BB-F349-9AE8-3CA5D331F114}"/>
+    <hyperlink ref="A162" r:id="rId159" display="http://www.pdbe.org/3jcm" xr:uid="{CEA6D395-B4A9-D941-A4EB-A24FB9872EF3}"/>
+    <hyperlink ref="A163" r:id="rId160" display="http://www.pdbe.org/5flc" xr:uid="{94FC8E90-E7BF-3446-B30D-BE111E36CE9F}"/>
+    <hyperlink ref="A164" r:id="rId161" display="http://www.pdbe.org/5fj6" xr:uid="{1F30FC86-AAAB-1341-830A-08263AAA9314}"/>
+    <hyperlink ref="A165" r:id="rId162" display="http://www.pdbe.org/5fkw" xr:uid="{B9555C13-FEDB-9540-9432-95150D39C2B1}"/>
+    <hyperlink ref="A166" r:id="rId163" display="http://www.pdbe.org/4ue4" xr:uid="{882A8725-4E13-014E-A065-68A3693D099B}"/>
+    <hyperlink ref="A167" r:id="rId164" display="http://www.pdbe.org/5a5t" xr:uid="{689BE5C2-C9F0-764A-B29C-F4C0BF3DF681}"/>
+    <hyperlink ref="A168" r:id="rId165" display="http://www.pdbe.org/3jaq" xr:uid="{FA337C49-C995-4E43-8C19-71F7BFC85149}"/>
+    <hyperlink ref="A169" r:id="rId166" display="http://www.pdbe.org/3j82" xr:uid="{CE863CEC-D91B-5A42-9D52-D541CB164873}"/>
+    <hyperlink ref="A170" r:id="rId167" display="http://www.pdbe.org/3j95" xr:uid="{8A557E04-ED3E-C64C-A0EC-FE7B68C5049C}"/>
+    <hyperlink ref="A171" r:id="rId168" display="http://www.pdbe.org/3j96" xr:uid="{EACC7290-B4ED-9B4F-844E-AD8BFCC75BE0}"/>
+    <hyperlink ref="A172" r:id="rId169" display="http://www.pdbe.org/4uxo" xr:uid="{EB7A1F12-6867-BF43-9A5B-5707363BA7EF}"/>
+    <hyperlink ref="A173" r:id="rId170" display="http://www.pdbe.org/4uxp" xr:uid="{E6169D10-3B1C-DF47-9D90-C45496F01A01}"/>
+    <hyperlink ref="A174" r:id="rId171" display="http://www.pdbe.org/4uxr" xr:uid="{FC9ECEC2-C819-3640-BC59-BD8212E679A4}"/>
+    <hyperlink ref="A175" r:id="rId172" display="http://www.pdbe.org/4uy0" xr:uid="{DDBFF9C0-B3AB-5C4A-8EDA-371CE5D95F5A}"/>
+    <hyperlink ref="A176" r:id="rId173" display="http://www.pdbe.org/4uqq" xr:uid="{72883B3B-D681-894A-83C5-30D61906B993}"/>
+    <hyperlink ref="A177" r:id="rId174" display="http://www.pdbe.org/3j5m" xr:uid="{C9D10936-B87D-4442-A6F1-64BE6F403CFA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added extra information on the new dataset and added a script to print the location of gaps in pdb structures
</commit_message>
<xml_diff>
--- a/data/candidates.xlsx
+++ b/data/candidates.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tneijen/Documents/gitdir/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFCAE92-9AD4-8242-A334-683925B257ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C03B7CA-CD40-D04D-B712-32927219EDCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="3720" windowWidth="24480" windowHeight="19240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14020" yWindow="2400" windowWidth="24480" windowHeight="19240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="candidates" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
     <sheet name="potential 5-8 angstrom" sheetId="4" r:id="rId4"/>
+    <sheet name="candidate list" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="clash_list_1" localSheetId="1">Sheet2!$D$2:$E$36</definedName>
@@ -46,7 +47,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{EBF0FFD7-3D05-3748-A6E2-F97DBDCB6DE6}" name="clashes1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/tneijen/Documents/Project/Dataset/5-8reso/clashes.csv" decimal="," thousands=".">
+    <textPr sourceFile="/Users/tneijen/Documents/Project/Dataset/5-8reso/clashes.csv" decimal="," thousands=".">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="781">
   <si>
     <t>EMDB ID</t>
   </si>
@@ -2271,13 +2272,142 @@
   </si>
   <si>
     <t>4 chains, contains N-ACETYL-D-GLUCOSAMINE (NAG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additional </t>
+  </si>
+  <si>
+    <t>chains</t>
+  </si>
+  <si>
+    <t>clashes</t>
+  </si>
+  <si>
+    <t>contains ADP</t>
+  </si>
+  <si>
+    <t>contains ATP</t>
+  </si>
+  <si>
+    <t>EMDB</t>
+  </si>
+  <si>
+    <t>resolution (Å)</t>
+  </si>
+  <si>
+    <t>EMD-4742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publication </t>
+  </si>
+  <si>
+    <t>doi: 10.1038/s41467-019-11772-y</t>
+  </si>
+  <si>
+    <t>EMD-3591</t>
+  </si>
+  <si>
+    <t>DOI: 10.1016/j.cell.2017.03.003</t>
+  </si>
+  <si>
+    <t>res count</t>
+  </si>
+  <si>
+    <t>EMD-9317</t>
+  </si>
+  <si>
+    <t>DOI: 10.7554/eLife.41215</t>
+  </si>
+  <si>
+    <t>unique chains</t>
+  </si>
+  <si>
+    <t>EMD-0375</t>
+  </si>
+  <si>
+    <t>DOI: 10.1016/j.celrep.2018.12.037</t>
+  </si>
+  <si>
+    <t>EMD-8695</t>
+  </si>
+  <si>
+    <t>DOI: 10.7554/eLife.27389</t>
+  </si>
+  <si>
+    <t>Contains TYS residue</t>
+  </si>
+  <si>
+    <t>EMD-9715</t>
+  </si>
+  <si>
+    <t>DOI: 10.1016/j.celrep.2018.11.071</t>
+  </si>
+  <si>
+    <t>EMD-20724</t>
+  </si>
+  <si>
+    <t>DOI: 10.2210/pdb6UC0/pdb</t>
+  </si>
+  <si>
+    <t>EMD-9537</t>
+  </si>
+  <si>
+    <t>EMD-7322</t>
+  </si>
+  <si>
+    <t>Contains Zn and Mg</t>
+  </si>
+  <si>
+    <t>contains MSE residue and Zn ion</t>
+  </si>
+  <si>
+    <t>DOI: 10.7554/eLife.34823</t>
+  </si>
+  <si>
+    <t>DOI: 10.1038/cr.2016.123</t>
+  </si>
+  <si>
+    <t>CSN–CRL2~N8 complex</t>
+  </si>
+  <si>
+    <t>RNA Polymerase I</t>
+  </si>
+  <si>
+    <t>imers of gyrase A in complex with DNA illuminate</t>
+  </si>
+  <si>
+    <t>HIV-1 Envelope trimer with antibodies</t>
+  </si>
+  <si>
+    <t>S3D-cofilin bound to an actin filament</t>
+  </si>
+  <si>
+    <t>SREBP-SCAP binding domains</t>
+  </si>
+  <si>
+    <t>Fdx/RbpA/σA-holo Complexes</t>
+  </si>
+  <si>
+    <t>GluN1/GluN2A NMDA recepto</t>
+  </si>
+  <si>
+    <t>ADP-bound N-ethylmaleimide sensitive factor</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>10.1038/nature14148</t>
+  </si>
+  <si>
+    <t>EMD-6205</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2430,6 +2560,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2802,7 +2938,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2814,6 +2950,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2874,11 +3012,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="2" xr16:uid="{DEC0D320-18C7-404B-BFD2-50D03D5167B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clashes" connectionId="2" xr16:uid="{DEC0D320-18C7-404B-BFD2-50D03D5167B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="clash_list_1" connectionId="1" xr16:uid="{8C6E6A6E-D13C-FE48-8399-68531717C107}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4086,7 +4224,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5040,8 +5178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7745B40B-F81E-7347-AA37-59DB198D8F7E}">
   <dimension ref="A1:O177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8076,4 +8214,364 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32B13DB-CD94-CE46-B3AD-0DCFA7BFED8B}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D1" t="s">
+        <v>739</v>
+      </c>
+      <c r="E1" t="s">
+        <v>753</v>
+      </c>
+      <c r="F1" t="s">
+        <v>750</v>
+      </c>
+      <c r="G1" t="s">
+        <v>744</v>
+      </c>
+      <c r="H1" t="s">
+        <v>738</v>
+      </c>
+      <c r="I1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2">
+        <v>275</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>3911</v>
+      </c>
+      <c r="G2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" t="s">
+        <v>766</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>747</v>
+      </c>
+      <c r="J2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B3" t="s">
+        <v>748</v>
+      </c>
+      <c r="C3">
+        <v>236</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>7778</v>
+      </c>
+      <c r="G3" t="s">
+        <v>330</v>
+      </c>
+      <c r="I3" t="s">
+        <v>749</v>
+      </c>
+      <c r="J3" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>688</v>
+      </c>
+      <c r="B4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4088</v>
+      </c>
+      <c r="G4" t="s">
+        <v>353</v>
+      </c>
+      <c r="I4" t="s">
+        <v>752</v>
+      </c>
+      <c r="J4" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B5" t="s">
+        <v>754</v>
+      </c>
+      <c r="C5">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>5274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>330</v>
+      </c>
+      <c r="H5" t="s">
+        <v>742</v>
+      </c>
+      <c r="I5" t="s">
+        <v>755</v>
+      </c>
+      <c r="J5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" t="s">
+        <v>756</v>
+      </c>
+      <c r="C6">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>3710</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>758</v>
+      </c>
+      <c r="I6" t="s">
+        <v>757</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B7" t="s">
+        <v>759</v>
+      </c>
+      <c r="C7">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3376</v>
+      </c>
+      <c r="G7" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" t="s">
+        <v>760</v>
+      </c>
+      <c r="J7" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>709</v>
+      </c>
+      <c r="B8" t="s">
+        <v>761</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2805</v>
+      </c>
+      <c r="G8" t="s">
+        <v>297</v>
+      </c>
+      <c r="H8" t="s">
+        <v>741</v>
+      </c>
+      <c r="I8" t="s">
+        <v>762</v>
+      </c>
+      <c r="J8" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>562</v>
+      </c>
+      <c r="B9" t="s">
+        <v>763</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>3084</v>
+      </c>
+      <c r="G9" t="s">
+        <v>368</v>
+      </c>
+      <c r="I9" t="s">
+        <v>768</v>
+      </c>
+      <c r="J9" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>653</v>
+      </c>
+      <c r="B10" t="s">
+        <v>764</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>3951</v>
+      </c>
+      <c r="G10" t="s">
+        <v>385</v>
+      </c>
+      <c r="H10" t="s">
+        <v>765</v>
+      </c>
+      <c r="I10" t="s">
+        <v>767</v>
+      </c>
+      <c r="J10" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>538</v>
+      </c>
+      <c r="B11" t="s">
+        <v>780</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>4482</v>
+      </c>
+      <c r="G11" t="s">
+        <v>778</v>
+      </c>
+      <c r="H11" t="s">
+        <v>741</v>
+      </c>
+      <c r="I11" t="s">
+        <v>779</v>
+      </c>
+      <c r="J11" t="s">
+        <v>777</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>